<commit_message>
MODIFIED: Refactor the code
</commit_message>
<xml_diff>
--- a/build/resources/test/UdemyData.xlsx
+++ b/build/resources/test/UdemyData.xlsx
@@ -365,7 +365,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,17 +488,16 @@
     <hyperlink ref="A7" r:id="rId10"/>
     <hyperlink ref="A9" r:id="rId11"/>
     <hyperlink ref="A11" r:id="rId12"/>
-    <hyperlink ref="B3:B12" r:id="rId13" display="Dinnu@247"/>
-    <hyperlink ref="B3" r:id="rId14"/>
-    <hyperlink ref="B4" r:id="rId15"/>
-    <hyperlink ref="B5" r:id="rId16"/>
+    <hyperlink ref="B3" r:id="rId13"/>
+    <hyperlink ref="B4" r:id="rId14"/>
+    <hyperlink ref="B5" r:id="rId15"/>
+    <hyperlink ref="B7" r:id="rId16"/>
     <hyperlink ref="B6" r:id="rId17"/>
-    <hyperlink ref="B7" r:id="rId18"/>
-    <hyperlink ref="B8" r:id="rId19"/>
-    <hyperlink ref="B9" r:id="rId20"/>
-    <hyperlink ref="B10" r:id="rId21"/>
-    <hyperlink ref="B11" r:id="rId22"/>
-    <hyperlink ref="B12" r:id="rId23"/>
+    <hyperlink ref="B8" r:id="rId18"/>
+    <hyperlink ref="B9" r:id="rId19"/>
+    <hyperlink ref="B10" r:id="rId20"/>
+    <hyperlink ref="B11" r:id="rId21"/>
+    <hyperlink ref="B12" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>